<commit_message>
updated for 2021-2022 season
</commit_message>
<xml_diff>
--- a/data/nfl_lookup_table.xlsx
+++ b/data/nfl_lookup_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richie/Dropbox/Records/Education/2019-20_BGSE_MScDataScience/Modules/DS-Trimester01/DataWarehousing/bgse19_dw_project2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cohen\Documents\nfl_optimizer-master\nfl_optimizer-master\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3CE78F-5EFE-7744-9364-40C7625E927D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6059668-1F9F-413C-98B0-1E0D0743E2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{F46A92DA-062D-F14B-9CE8-C125F7030FA4}"/>
+    <workbookView xWindow="28680" yWindow="-5985" windowWidth="29040" windowHeight="16440" xr2:uid="{F46A92DA-062D-F14B-9CE8-C125F7030FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -276,9 +279,6 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>WAS</t>
-  </si>
-  <si>
     <t>Washington</t>
   </si>
   <si>
@@ -345,9 +345,6 @@
     <t>NFC</t>
   </si>
   <si>
-    <t>********</t>
-  </si>
-  <si>
     <t>Oakland Alameda Coliseum</t>
   </si>
   <si>
@@ -538,6 +535,12 @@
   </si>
   <si>
     <t>New Orleans, Louisiana</t>
+  </si>
+  <si>
+    <t>Football Team</t>
+  </si>
+  <si>
+    <t>WSH</t>
   </si>
 </sst>
 </file>
@@ -901,21 +904,21 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,13 +938,13 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -952,23 +955,23 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H2" t="str">
         <f>A2&amp;".png"</f>
         <v>ARI.png</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -979,23 +982,23 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H33" si="0">A3&amp;".png"</f>
+        <f t="shared" ref="H3:H32" si="0">A3&amp;".png"</f>
         <v>ATL.png</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1006,23 +1009,23 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>BAL.png</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1033,23 +1036,23 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
         <v>91</v>
       </c>
-      <c r="E5" t="s">
-        <v>92</v>
-      </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>BUF.png</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1060,23 +1063,23 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>CAR.png</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1087,50 +1090,50 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>CHI.png</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>94</v>
       </c>
-      <c r="F7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>CHI.png</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>95</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>96</v>
       </c>
-      <c r="C8" t="s">
-        <v>97</v>
-      </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>CIN.png</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1141,77 +1144,77 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>CLE.png</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
         <v>89</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>DAL.png</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
         <v>87</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>DEN.png</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1222,23 +1225,23 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>DET.png</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1249,23 +1252,23 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>GB.png</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1276,23 +1279,23 @@
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>HOU.png</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1303,23 +1306,23 @@
         <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>IND.png</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1330,23 +1333,23 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>JAX.png</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1357,77 +1360,77 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>KC.png</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>99</v>
       </c>
-      <c r="F17" t="s">
-        <v>156</v>
-      </c>
-      <c r="G17" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>KC.png</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>100</v>
-      </c>
-      <c r="B18" t="s">
-        <v>101</v>
       </c>
       <c r="C18" t="s">
         <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
         <v>LAC.png</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
         <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
         <v>LAR.png</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1438,23 +1441,23 @@
         <v>49</v>
       </c>
       <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
         <v>91</v>
       </c>
-      <c r="E20" t="s">
-        <v>92</v>
-      </c>
       <c r="F20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
         <v>MIA.png</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1465,23 +1468,23 @@
         <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
         <v>MIN.png</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1492,23 +1495,23 @@
         <v>55</v>
       </c>
       <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
         <v>91</v>
       </c>
-      <c r="E22" t="s">
-        <v>92</v>
-      </c>
       <c r="F22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
         <v>NE.png</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1519,23 +1522,23 @@
         <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
         <v>NO.png</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1546,23 +1549,23 @@
         <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
         <v>NYG.png</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1573,23 +1576,23 @@
         <v>63</v>
       </c>
       <c r="D25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" t="s">
         <v>91</v>
       </c>
-      <c r="E25" t="s">
-        <v>92</v>
-      </c>
       <c r="F25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
         <v>NYJ.png</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1600,23 +1603,23 @@
         <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
         <v>OAK.png</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1627,23 +1630,23 @@
         <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
         <v>PHI.png</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -1654,50 +1657,50 @@
         <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
         <v>PIT.png</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29" t="s">
         <v>126</v>
       </c>
-      <c r="D29" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" t="s">
-        <v>163</v>
-      </c>
-      <c r="G29" t="s">
-        <v>128</v>
-      </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
         <v>SF.png</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1708,106 +1711,106 @@
         <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
         <v>SEA.png</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
         <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>84</v>
       </c>
       <c r="C31" t="s">
         <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
         <v>TB.png</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" t="s">
         <v>85</v>
-      </c>
-      <c r="B32" t="s">
-        <v>86</v>
       </c>
       <c r="C32" t="s">
         <v>80</v>
       </c>
       <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" t="s">
+        <v>164</v>
+      </c>
+      <c r="G32" t="s">
+        <v>136</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>TEN.png</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" t="s">
         <v>91</v>
       </c>
-      <c r="E32" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" t="s">
-        <v>166</v>
-      </c>
-      <c r="G32" t="s">
-        <v>138</v>
-      </c>
-      <c r="H32" t="str">
-        <f t="shared" si="0"/>
-        <v>TEN.png</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" t="s">
-        <v>92</v>
-      </c>
       <c r="F33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>WAS.png</v>
+        <f t="shared" ref="H33" si="1">A33&amp;".png"</f>
+        <v>WSH.png</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E33">
-    <sortCondition ref="B2:B33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E32">
+    <sortCondition ref="B2:B32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>